<commit_message>
1) Added Asserts in test method 2) Edit rule test script is updated. 3) Delete rule updated 4) Add new rule updated 5) Test data updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Test Data WifiAnalyser.xlsx
+++ b/src/test/resources/TestData/Test Data WifiAnalyser.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Add new rule" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Delete Rule" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Edit Rule" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="52">
   <si>
     <t xml:space="preserve">Rule Name</t>
   </si>
@@ -128,19 +129,55 @@
     <t xml:space="preserve">Count of Clientcount</t>
   </si>
   <si>
+    <t xml:space="preserve">Timestamp Rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MINOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-03-03 18:56:55.177+0530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter by AP Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA_6F_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter by {APNAME}</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rule Names</t>
   </si>
   <si>
-    <t xml:space="preserve">Test rule timestamp </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Advance Rule Test </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filter Status Test Rule </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FilterROLE Test Rule </t>
+    <t xml:space="preserve">Notification Rule Message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIR-CAP3702I-D-K9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-03-09 18:56:55.177+0530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timestamp rule</t>
   </si>
 </sst>
 </file>
@@ -235,12 +272,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -252,14 +289,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -268,23 +297,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -305,38 +326,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.72959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.7602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="17.9081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -345,10 +365,10 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -366,131 +386,213 @@
       <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    <row r="2" customFormat="false" ht="57.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="J2" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+    <row r="3" customFormat="false" ht="59.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="J3" s="6" t="n">
+      <c r="I3" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="J3" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="6" t="s">
+      <c r="K3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+    <row r="4" customFormat="false" ht="52.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="6" t="n">
+      <c r="I4" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="J4" s="6" t="n">
+      <c r="J4" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="6" t="s">
+      <c r="K4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="52.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -512,42 +614,327 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.9234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.0510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.2295918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.7448979591837"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.0255102040816"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.3214285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.0255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="27.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="61.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="J3" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="36.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="44.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="44.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>39</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Login test script completed with Asserts.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Test Data WifiAnalyser.xlsx
+++ b/src/test/resources/TestData/Test Data WifiAnalyser.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login credentials" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="64">
   <si>
     <t xml:space="preserve">User name</t>
   </si>
@@ -82,106 +82,121 @@
     <t xml:space="preserve">Notification Rule Message:  </t>
   </si>
   <si>
+    <t xml:space="preserve">Second Rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NORMAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wlc_client_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANDWIDTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> %{aggregation} %{metric} %{expression} %{comparator} %{triggervalue} %{timewindow}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bandwidth rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRITICAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">==</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wlc_ap_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APSLOTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fourth rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMPORTANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APMODEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIR-CAP3702I-N-K9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLIENTCOUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of Clientcount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fifth rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MINOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-03-03 18:56:55.177+0530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sixth rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA_6F_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter by {APNAME}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rule Names</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bandwidth Rule</t>
   </si>
   <si>
-    <t xml:space="preserve">NORMAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wlc_client_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BANDWIDTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;=</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> %{aggregation} %{metric} %{expression} %{comparator} %{triggervalue} %{timewindow}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bandwidth rule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Count of users</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRITICAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">==</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wlc_ap_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APSLOTS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Count of clientcount</t>
   </si>
   <si>
-    <t xml:space="preserve">IMPORTANT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APMODEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIR-CAP3702I-N-K9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLIENTCOUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Count of Clientcount</t>
-  </si>
-  <si>
     <t xml:space="preserve">Timestamp Rule</t>
   </si>
   <si>
-    <t xml:space="preserve">MINOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-03-03 18:56:55.177+0530</t>
-  </si>
-  <si>
     <t xml:space="preserve">Filter by AP Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AA_6F_04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filter by {APNAME}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rule Names</t>
   </si>
   <si>
     <t xml:space="preserve">Notification Rule Message</t>
@@ -369,14 +384,15 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,26 +476,25 @@
   </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.7397959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -602,30 +617,30 @@
         <v>28</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="52.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>34</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>26</v>
@@ -643,24 +658,24 @@
         <v>28</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="52.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>24</v>
@@ -689,34 +704,34 @@
     </row>
     <row r="6" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>24</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>27</v>
@@ -725,7 +740,7 @@
         <v>28</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -752,38 +767,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -810,18 +825,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -862,12 +877,12 @@
         <v>17</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="61.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>31</v>
@@ -894,7 +909,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>27</v>
@@ -903,30 +918,30 @@
         <v>28</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>26</v>
@@ -944,12 +959,12 @@
         <v>28</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="36.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>20</v>
@@ -990,19 +1005,19 @@
     </row>
     <row r="5" customFormat="false" ht="44.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>24</v>
@@ -1014,7 +1029,7 @@
         <v>26</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="J5" s="8" t="n">
         <v>20</v>
@@ -1026,39 +1041,39 @@
         <v>28</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="44.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>24</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>27</v>
@@ -1067,7 +1082,7 @@
         <v>28</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code review changes :
1)Login test script: verify invalid login by error msg.
2)Add new rule test script : write Login method in @BeforeMethod
3)Pass property file name to Reading property class.
4)BasePage :open browser code is written in launchBrowser() method
5)change in ReadingProperty file - loadProperty() is removed and code is
shifted to the constructor of ReadingProperty file.
6) isElementPresent() - logic is changed
7) Separate dataprovider class is created
8) SleepMethod() is written for thread.sleep()
9) verifyContainsText(), verifyContainsTextbyboolean() methods are
shifted to BasePage class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Test Data WifiAnalyser.xlsx
+++ b/src/test/resources/TestData/Test Data WifiAnalyser.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="66">
   <si>
     <t xml:space="preserve">User name</t>
   </si>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Notification Rule Message:  </t>
   </si>
   <si>
-    <t xml:space="preserve">Automation test</t>
+    <t xml:space="preserve">Third test</t>
   </si>
   <si>
     <t xml:space="preserve">NORMAL</t>
@@ -118,15 +118,87 @@
     <t xml:space="preserve">Bandwidth rule</t>
   </si>
   <si>
+    <t xml:space="preserve">Fourth rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRITICAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">==</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wlc_ap_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APSLOTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fifth rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMPORTANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APMODEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIR-CAP3702I-N-K9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLIENTCOUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of Clientcount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sixth rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MINOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-03-30 12:00:55.177+0530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timestamp rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seventh rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA_6F_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter by {APNAME}</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rule Names</t>
   </si>
   <si>
     <t xml:space="preserve">Bandwidth Rule</t>
   </si>
   <si>
-    <t xml:space="preserve">Count of users</t>
-  </si>
-  <si>
     <t xml:space="preserve">Count of clientcount</t>
   </si>
   <si>
@@ -139,64 +211,16 @@
     <t xml:space="preserve">Notification Rule Message</t>
   </si>
   <si>
-    <t xml:space="preserve">CRITICAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">==</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wlc_ap_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APSLOTS</t>
-  </si>
-  <si>
     <t xml:space="preserve">100</t>
   </si>
   <si>
-    <t xml:space="preserve">IMPORTANT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APMODEL</t>
-  </si>
-  <si>
     <t xml:space="preserve">AIR-CAP3702I-D-K9</t>
   </si>
   <si>
-    <t xml:space="preserve">CLIENTCOUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Count of Clientcount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timestamp</t>
-  </si>
-  <si>
     <t xml:space="preserve">2017-03-09 18:56:55.177+0530</t>
   </si>
   <si>
     <t xml:space="preserve">5000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timestamp rule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AA_6F_04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filter by {APNAME}</t>
   </si>
 </sst>
 </file>
@@ -299,7 +323,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -324,24 +348,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -372,14 +388,14 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -394,45 +410,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="C2" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="6" t="n">
         <v>123</v>
       </c>
-      <c r="C3" s="5" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="C3" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="5" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="n">
+      <c r="A5" s="3"/>
+      <c r="B5" s="6" t="n">
         <v>123</v>
       </c>
-      <c r="C5" s="5" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="C5" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -440,21 +452,19 @@
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="B6" s="3"/>
+      <c r="C6" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="C7" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -465,8 +475,7 @@
       <c r="B8" s="4" t="n">
         <v>123</v>
       </c>
-      <c r="C8" s="5" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C8" s="5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -493,27 +502,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1173469387755"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.9183673469388"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0867346938776"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -550,52 +559,216 @@
       <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="57.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="10" t="n">
+      <c r="I2" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="10" t="n">
+      <c r="J2" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="7" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="J3" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -622,38 +795,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3061224489796"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>32</v>
+      <c r="A2" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>33</v>
+      <c r="A3" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>34</v>
+      <c r="A4" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>35</v>
+      <c r="A5" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
-        <v>36</v>
+      <c r="A6" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -675,22 +848,24 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.765306122449"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6887755102041"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.7397959183673"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
@@ -728,216 +903,216 @@
       <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="61.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="61.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="B2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="E2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="J3" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="36.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="10" t="s">
+      <c r="D4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="44.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="44.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="11" t="s">
+      <c r="H6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="J3" s="10" t="n">
-        <v>30</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="36.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="J4" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="44.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="44.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="10" t="s">
+      <c r="M6" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>